<commit_message>
zdechov & other new/fixed results
</commit_message>
<xml_diff>
--- a/processor/outputTemplate.xlsx
+++ b/processor/outputTemplate.xlsx
@@ -46,10 +46,10 @@
     <t xml:space="preserve">Klobucká kola</t>
   </si>
   <si>
-    <t xml:space="preserve">Zděchov</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bratřejov</t>
+    <t xml:space="preserve">Zděchovský krpál</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bratřejovské kotáry</t>
   </si>
   <si>
     <t xml:space="preserve">Polanský duatlonek</t>
@@ -370,11 +370,11 @@
   </sheetPr>
   <dimension ref="A2:AD8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S4" activeCellId="0" sqref="S4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.82421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.84765625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25"/>
@@ -719,6 +719,8 @@
     <hyperlink ref="E4" r:id="rId1" display="Hradní okruh"/>
     <hyperlink ref="G4" r:id="rId2" display="O pohár starosty obce Lačnov"/>
     <hyperlink ref="K4" r:id="rId3" display="Klobucká kola"/>
+    <hyperlink ref="O4" r:id="rId4" display="Zděchovský krpál"/>
+    <hyperlink ref="S4" r:id="rId5" display="Bratřejovské kotáry"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.329861111111111" right="0.329861111111111" top="0.329861111111111" bottom="0.329861111111111" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
adding 2023, race #1
</commit_message>
<xml_diff>
--- a/processor/outputTemplate.xlsx
+++ b/processor/outputTemplate.xlsx
@@ -11,8 +11,8 @@
     <sheet name="Template" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Template!$B$2:$AD$175</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Template!$B$2:$AD$200</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Template!$B$2:$AD$175</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">Template!$B$2:$S$71</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">Template!$B$2:$S$50</definedName>
   </definedNames>
@@ -40,15 +40,15 @@
     <t xml:space="preserve">Hradní okruh</t>
   </si>
   <si>
+    <t xml:space="preserve">Klobucká kola</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zděchovský krpál</t>
+  </si>
+  <si>
     <t xml:space="preserve">O pohár starosty obce Lačnov</t>
   </si>
   <si>
-    <t xml:space="preserve">Klobucká kola</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zděchovský krpál</t>
-  </si>
-  <si>
     <t xml:space="preserve">Bratřejovské kotáry</t>
   </si>
   <si>
@@ -58,25 +58,25 @@
     <t xml:space="preserve">Ploština - Memoriál Josefa Valčíka</t>
   </si>
   <si>
-    <t xml:space="preserve">28. 5.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4. 6.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25. 6.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2. 7.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13. 8.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">17. 9.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8. 10.</t>
+    <t xml:space="preserve">27. 5.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24. 6.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. 7.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15. 7.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12. 8.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16. 9.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7. 10.</t>
   </si>
   <si>
     <t xml:space="preserve">Jméno</t>
@@ -158,19 +158,16 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="238"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="238"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="238"/>
     </font>
     <font>
       <b val="true"/>
@@ -300,72 +297,76 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -382,321 +383,321 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
   <dimension ref="A2:AD8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J21" activeCellId="0" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8671875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="32.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1021" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="4.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="32.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1021" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="AD2" s="2" t="s">
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="AD2" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4" t="s">
+      <c r="F4" s="5"/>
+      <c r="G4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4" t="s">
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4" t="s">
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="4"/>
-      <c r="Q4" s="4"/>
-      <c r="R4" s="4"/>
-      <c r="S4" s="4" t="s">
+      <c r="P4" s="5"/>
+      <c r="Q4" s="5"/>
+      <c r="R4" s="5"/>
+      <c r="S4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="T4" s="4"/>
-      <c r="U4" s="4"/>
-      <c r="V4" s="4"/>
-      <c r="W4" s="4" t="s">
+      <c r="T4" s="5"/>
+      <c r="U4" s="5"/>
+      <c r="V4" s="5"/>
+      <c r="W4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="X4" s="4"/>
-      <c r="Y4" s="4"/>
-      <c r="Z4" s="4"/>
-      <c r="AA4" s="4" t="s">
+      <c r="X4" s="5"/>
+      <c r="Y4" s="5"/>
+      <c r="Z4" s="5"/>
+      <c r="AA4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="AB4" s="4"/>
-      <c r="AC4" s="4"/>
-      <c r="AD4" s="4"/>
+      <c r="AB4" s="5"/>
+      <c r="AC4" s="5"/>
+      <c r="AD4" s="5"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="6" t="s">
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6" t="s">
+      <c r="F5" s="7"/>
+      <c r="G5" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6" t="s">
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="6"/>
-      <c r="O5" s="6" t="s">
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="P5" s="6"/>
-      <c r="Q5" s="6"/>
-      <c r="R5" s="6"/>
-      <c r="S5" s="6" t="s">
+      <c r="P5" s="7"/>
+      <c r="Q5" s="7"/>
+      <c r="R5" s="7"/>
+      <c r="S5" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="T5" s="6"/>
-      <c r="U5" s="6"/>
-      <c r="V5" s="6"/>
-      <c r="W5" s="6" t="s">
+      <c r="T5" s="7"/>
+      <c r="U5" s="7"/>
+      <c r="V5" s="7"/>
+      <c r="W5" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="X5" s="6"/>
-      <c r="Y5" s="6"/>
-      <c r="Z5" s="6"/>
-      <c r="AA5" s="6" t="s">
+      <c r="X5" s="7"/>
+      <c r="Y5" s="7"/>
+      <c r="Z5" s="7"/>
+      <c r="AA5" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="AB5" s="6"/>
-      <c r="AC5" s="6"/>
-      <c r="AD5" s="6"/>
+      <c r="AB5" s="7"/>
+      <c r="AC5" s="7"/>
+      <c r="AD5" s="7"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7"/>
-      <c r="B6" s="8" t="s">
+      <c r="A6" s="8"/>
+      <c r="B6" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="F6" s="9"/>
-      <c r="G6" s="10" t="s">
+      <c r="F6" s="10"/>
+      <c r="G6" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="H6" s="10"/>
-      <c r="I6" s="9" t="s">
+      <c r="H6" s="11"/>
+      <c r="I6" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="J6" s="9"/>
-      <c r="K6" s="10" t="s">
+      <c r="J6" s="10"/>
+      <c r="K6" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="L6" s="10"/>
-      <c r="M6" s="9" t="s">
+      <c r="L6" s="11"/>
+      <c r="M6" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="N6" s="9"/>
-      <c r="O6" s="10" t="s">
+      <c r="N6" s="10"/>
+      <c r="O6" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="P6" s="10"/>
-      <c r="Q6" s="9" t="s">
+      <c r="P6" s="11"/>
+      <c r="Q6" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="R6" s="9"/>
-      <c r="S6" s="10" t="s">
+      <c r="R6" s="10"/>
+      <c r="S6" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="T6" s="10"/>
-      <c r="U6" s="9" t="s">
+      <c r="T6" s="11"/>
+      <c r="U6" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="V6" s="9"/>
-      <c r="W6" s="10" t="s">
+      <c r="V6" s="10"/>
+      <c r="W6" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="X6" s="10"/>
-      <c r="Y6" s="9" t="s">
+      <c r="X6" s="11"/>
+      <c r="Y6" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="Z6" s="9"/>
-      <c r="AA6" s="10" t="s">
+      <c r="Z6" s="10"/>
+      <c r="AA6" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="AB6" s="10"/>
-      <c r="AC6" s="9" t="s">
+      <c r="AB6" s="11"/>
+      <c r="AC6" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="AD6" s="9"/>
+      <c r="AD6" s="10"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="7"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="11" t="s">
+      <c r="A7" s="8"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F7" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="G7" s="12" t="s">
+      <c r="F7" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="G7" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="H7" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="I7" s="11" t="s">
+      <c r="H7" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="I7" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="J7" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="K7" s="12" t="s">
+      <c r="J7" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="K7" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="L7" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="M7" s="11" t="s">
+      <c r="L7" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="M7" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="N7" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="O7" s="12" t="s">
+      <c r="N7" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="O7" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="P7" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q7" s="11" t="s">
+      <c r="P7" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q7" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="R7" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="S7" s="12" t="s">
+      <c r="R7" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="S7" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="T7" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="U7" s="11" t="s">
+      <c r="T7" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="U7" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="V7" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="W7" s="12" t="s">
+      <c r="V7" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="W7" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="X7" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="Y7" s="11" t="s">
+      <c r="X7" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y7" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="Z7" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="AA7" s="12" t="s">
+      <c r="Z7" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="AA7" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="AB7" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="AC7" s="11" t="s">
+      <c r="AB7" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="AC7" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="AD7" s="11" t="s">
+      <c r="AD7" s="12" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="7"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="12" t="s">
+      <c r="A8" s="8"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="E8" s="11"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="16"/>
-      <c r="M8" s="11"/>
-      <c r="N8" s="15"/>
-      <c r="O8" s="12"/>
-      <c r="P8" s="16"/>
-      <c r="Q8" s="11"/>
-      <c r="R8" s="15"/>
-      <c r="S8" s="12"/>
-      <c r="T8" s="16"/>
-      <c r="U8" s="11"/>
-      <c r="V8" s="15"/>
-      <c r="W8" s="12"/>
-      <c r="X8" s="16"/>
-      <c r="Y8" s="11"/>
-      <c r="Z8" s="15"/>
-      <c r="AA8" s="12"/>
-      <c r="AB8" s="16"/>
-      <c r="AC8" s="11"/>
-      <c r="AD8" s="15"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="17"/>
+      <c r="M8" s="12"/>
+      <c r="N8" s="16"/>
+      <c r="O8" s="13"/>
+      <c r="P8" s="17"/>
+      <c r="Q8" s="12"/>
+      <c r="R8" s="16"/>
+      <c r="S8" s="13"/>
+      <c r="T8" s="17"/>
+      <c r="U8" s="12"/>
+      <c r="V8" s="16"/>
+      <c r="W8" s="13"/>
+      <c r="X8" s="17"/>
+      <c r="Y8" s="12"/>
+      <c r="Z8" s="16"/>
+      <c r="AA8" s="13"/>
+      <c r="AB8" s="17"/>
+      <c r="AC8" s="12"/>
+      <c r="AD8" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="32">
@@ -736,9 +737,9 @@
   <hyperlinks>
     <hyperlink ref="AD2" r:id="rId1" display="https://vkct.webnode.cz/"/>
     <hyperlink ref="E4" r:id="rId2" display="Hradní okruh"/>
-    <hyperlink ref="G4" r:id="rId3" display="O pohár starosty obce Lačnov"/>
-    <hyperlink ref="K4" r:id="rId4" display="Klobucká kola"/>
-    <hyperlink ref="O4" r:id="rId5" display="Zděchovský krpál"/>
+    <hyperlink ref="G4" r:id="rId3" display="Klobucká kola"/>
+    <hyperlink ref="K4" r:id="rId4" display="Zděchovský krpál"/>
+    <hyperlink ref="O4" r:id="rId5" display="O pohár starosty obce Lačnov"/>
     <hyperlink ref="S4" r:id="rId6" display="Bratřejovské kotáry"/>
     <hyperlink ref="AA4" r:id="rId7" display="Ploština - Memoriál Josefa Valčíka"/>
   </hyperlinks>

</xml_diff>

<commit_message>
1 dva zavody 2025
</commit_message>
<xml_diff>
--- a/processor/outputTemplate.xlsx
+++ b/processor/outputTemplate.xlsx
@@ -8,13 +8,13 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Template" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Template" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Template!$B$2:$AD$175</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Template!$B$2:$AD$200</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">Template!$B$2:$S$71</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">Template!$B$2:$S$50</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Template!$B$2:$V$175</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Template!$B$2:$V$200</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">Template!$B$2:$O$71</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">Template!$B$2:$O$50</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="29">
   <si>
     <t xml:space="preserve">Force Valašskokarpatská cyklotour</t>
   </si>
@@ -43,42 +43,30 @@
     <t xml:space="preserve">Klobucká kola</t>
   </si>
   <si>
-    <t xml:space="preserve">Zděchovský krpál</t>
-  </si>
-  <si>
     <t xml:space="preserve">Bratřejovské kotáry</t>
   </si>
   <si>
     <t xml:space="preserve">O pohár starosty obce Lačnov</t>
   </si>
   <si>
-    <t xml:space="preserve">Polanský duatlonek</t>
-  </si>
-  <si>
     <t xml:space="preserve">Ploština - Memoriál Josefa Valčíka</t>
   </si>
   <si>
-    <t xml:space="preserve">25. 5.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15. 6.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22. 6.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10. 8.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24. 8.</t>
+    <t xml:space="preserve">24. 5.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14. 6.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9. 8.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20. 9.</t>
   </si>
   <si>
     <t xml:space="preserve">28. 9.</t>
   </si>
   <si>
-    <t xml:space="preserve">5. 10.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Jméno</t>
   </si>
   <si>
@@ -97,12 +85,6 @@
     <t xml:space="preserve">pořadí po 2. závodě</t>
   </si>
   <si>
-    <t xml:space="preserve">3. závod</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pořadí po 3. závodě</t>
-  </si>
-  <si>
     <t xml:space="preserve">4. závod</t>
   </si>
   <si>
@@ -119,12 +101,6 @@
   </si>
   <si>
     <t xml:space="preserve">pořadí po 6. závodě</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7. závod</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pořadí po 7. závodě</t>
   </si>
   <si>
     <t xml:space="preserve">pořadí</t>
@@ -146,7 +122,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -180,14 +156,6 @@
     <font>
       <b val="true"/>
       <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -254,7 +222,7 @@
       <left style="thin"/>
       <right style="thin"/>
       <top/>
-      <bottom/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -318,47 +286,47 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -382,23 +350,131 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A2:AD8"/>
+  <dimension ref="A2:V8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="W6" activeCellId="0" sqref="W6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K1" activeCellId="0" sqref="K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8671875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.8671875" defaultRowHeight="13.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="4.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="32.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1021" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1016" min="1013" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16380" min="16377" style="0" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16381" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -413,7 +489,7 @@
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
-      <c r="AD2" s="3" t="s">
+      <c r="V2" s="3" t="s">
         <v>1</v>
       </c>
     </row>
@@ -430,7 +506,7 @@
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E4" s="5" t="s">
         <v>3</v>
       </c>
@@ -459,127 +535,87 @@
       <c r="T4" s="5"/>
       <c r="U4" s="5"/>
       <c r="V4" s="5"/>
-      <c r="W4" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="X4" s="5"/>
-      <c r="Y4" s="5"/>
-      <c r="Z4" s="5"/>
-      <c r="AA4" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="AB4" s="5"/>
-      <c r="AC4" s="5"/>
-      <c r="AD4" s="5"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
       <c r="E5" s="7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F5" s="7"/>
       <c r="G5" s="7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
       <c r="K5" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="L5" s="7"/>
       <c r="M5" s="7"/>
       <c r="N5" s="7"/>
       <c r="O5" s="7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="P5" s="7"/>
       <c r="Q5" s="7"/>
       <c r="R5" s="7"/>
       <c r="S5" s="7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="T5" s="7"/>
       <c r="U5" s="7"/>
       <c r="V5" s="7"/>
-      <c r="W5" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="X5" s="7"/>
-      <c r="Y5" s="7"/>
-      <c r="Z5" s="7"/>
-      <c r="AA5" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="AB5" s="7"/>
-      <c r="AC5" s="7"/>
-      <c r="AD5" s="7"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="8"/>
       <c r="B6" s="9" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="F6" s="10"/>
       <c r="G6" s="11" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="H6" s="11"/>
       <c r="I6" s="10" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="J6" s="10"/>
       <c r="K6" s="11" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="L6" s="11"/>
       <c r="M6" s="10" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="N6" s="10"/>
       <c r="O6" s="11" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="P6" s="11"/>
       <c r="Q6" s="10" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="R6" s="10"/>
       <c r="S6" s="11" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="T6" s="11"/>
       <c r="U6" s="10" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="V6" s="10"/>
-      <c r="W6" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="X6" s="11"/>
-      <c r="Y6" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="Z6" s="10"/>
-      <c r="AA6" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="AB6" s="11"/>
-      <c r="AC6" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="AD6" s="10"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="8"/>
@@ -587,82 +623,58 @@
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
       <c r="E7" s="12" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="G7" s="13" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="H7" s="13" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="I7" s="12" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="J7" s="12" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="K7" s="13" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="L7" s="13" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="M7" s="12" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="N7" s="12" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="O7" s="13" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="P7" s="13" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="Q7" s="12" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="R7" s="12" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="S7" s="13" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="T7" s="13" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="U7" s="12" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="V7" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="W7" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="X7" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="Y7" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="Z7" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="AA7" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="AB7" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="AC7" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="AD7" s="12" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -670,7 +682,7 @@
       <c r="B8" s="14"/>
       <c r="C8" s="15"/>
       <c r="D8" s="13" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="E8" s="12"/>
       <c r="F8" s="16"/>
@@ -690,17 +702,9 @@
       <c r="T8" s="17"/>
       <c r="U8" s="12"/>
       <c r="V8" s="16"/>
-      <c r="W8" s="13"/>
-      <c r="X8" s="17"/>
-      <c r="Y8" s="12"/>
-      <c r="Z8" s="16"/>
-      <c r="AA8" s="13"/>
-      <c r="AB8" s="17"/>
-      <c r="AC8" s="12"/>
-      <c r="AD8" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="32">
+  <mergeCells count="24">
     <mergeCell ref="B2:J2"/>
     <mergeCell ref="B3:J3"/>
     <mergeCell ref="E4:F4"/>
@@ -708,15 +712,11 @@
     <mergeCell ref="K4:N4"/>
     <mergeCell ref="O4:R4"/>
     <mergeCell ref="S4:V4"/>
-    <mergeCell ref="W4:Z4"/>
-    <mergeCell ref="AA4:AD4"/>
     <mergeCell ref="E5:F5"/>
     <mergeCell ref="G5:J5"/>
     <mergeCell ref="K5:N5"/>
     <mergeCell ref="O5:R5"/>
     <mergeCell ref="S5:V5"/>
-    <mergeCell ref="W5:Z5"/>
-    <mergeCell ref="AA5:AD5"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="D6:D7"/>
@@ -729,19 +729,14 @@
     <mergeCell ref="Q6:R6"/>
     <mergeCell ref="S6:T6"/>
     <mergeCell ref="U6:V6"/>
-    <mergeCell ref="W6:X6"/>
-    <mergeCell ref="Y6:Z6"/>
-    <mergeCell ref="AA6:AB6"/>
-    <mergeCell ref="AC6:AD6"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="AD2" r:id="rId1" display="https://vkct.webnode.cz/"/>
+    <hyperlink ref="V2" r:id="rId1" display="https://vkct.webnode.cz/"/>
     <hyperlink ref="E4" r:id="rId2" display="Hradní okruh"/>
     <hyperlink ref="G4" r:id="rId3" display="Klobucká kola"/>
-    <hyperlink ref="K4" r:id="rId4" display="Zděchovský krpál"/>
-    <hyperlink ref="O4" r:id="rId5" display="Bratřejovské kotáry"/>
-    <hyperlink ref="S4" r:id="rId6" display="O pohár starosty obce Lačnov"/>
-    <hyperlink ref="AA4" r:id="rId7" display="Ploština - Memoriál Josefa Valčíka"/>
+    <hyperlink ref="K4" r:id="rId4" display="Bratřejovské kotáry"/>
+    <hyperlink ref="O4" r:id="rId5" display="O pohár starosty obce Lačnov"/>
+    <hyperlink ref="S4" r:id="rId6" display="Ploština - Memoriál Josefa Valčíka"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.329861111111111" right="0.329861111111111" top="0.329861111111111" bottom="0.329861111111111" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>